<commit_message>
Deleting un useful files
</commit_message>
<xml_diff>
--- a/Selenium with CSharp/Selenium with CSharp/TestData2.xlsx
+++ b/Selenium with CSharp/Selenium with CSharp/TestData2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.mohamed\Documents\GitHub\Selenium-c-\Selenium with CSharp\Selenium with CSharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6E4523A-3A96-472C-9152-E04E7BA905D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6718300F-9CCF-4103-A51D-2C96438279FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
   </bookViews>
@@ -72,25 +72,25 @@
     <t>Cerner</t>
   </si>
   <si>
-    <t>Pharmacy_h4Sept</t>
-  </si>
-  <si>
-    <t>p19934223</t>
-  </si>
-  <si>
-    <t>Alignment Project 19</t>
-  </si>
-  <si>
-    <t>TestAutomation_6Sep</t>
-  </si>
-  <si>
-    <t>A224119933</t>
-  </si>
-  <si>
-    <t>Facility_h22493355</t>
-  </si>
-  <si>
-    <t>h22493355</t>
+    <t>TestAutomation_8Sep</t>
+  </si>
+  <si>
+    <t>A2241199332</t>
+  </si>
+  <si>
+    <t>Facility_h224933552</t>
+  </si>
+  <si>
+    <t>h224933552</t>
+  </si>
+  <si>
+    <t>Pharmacy_h8Sept</t>
+  </si>
+  <si>
+    <t>p199342232</t>
+  </si>
+  <si>
+    <t>Alignment Project 192</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,28 +714,28 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updata Test data driven in order to Try and update the script
</commit_message>
<xml_diff>
--- a/Selenium with CSharp/Selenium with CSharp/TestData2.xlsx
+++ b/Selenium with CSharp/Selenium with CSharp/TestData2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.mohamed\Documents\GitHub\Selenium-c-\Selenium with CSharp\Selenium with CSharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6718300F-9CCF-4103-A51D-2C96438279FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93105C22-09EF-4413-9186-CD68392DB067}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
   </bookViews>
@@ -72,18 +72,6 @@
     <t>Cerner</t>
   </si>
   <si>
-    <t>TestAutomation_8Sep</t>
-  </si>
-  <si>
-    <t>A2241199332</t>
-  </si>
-  <si>
-    <t>Facility_h224933552</t>
-  </si>
-  <si>
-    <t>h224933552</t>
-  </si>
-  <si>
     <t>Pharmacy_h8Sept</t>
   </si>
   <si>
@@ -91,6 +79,18 @@
   </si>
   <si>
     <t>Alignment Project 192</t>
+  </si>
+  <si>
+    <t>TestAutomation_8Septt</t>
+  </si>
+  <si>
+    <t>A224119933241</t>
+  </si>
+  <si>
+    <t>Facility_h224933552q</t>
+  </si>
+  <si>
+    <t>h224933552q</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,28 +714,28 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="F5" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maintaining the script in order to improve the steps and adding two methods in test base class to handle waiting
</commit_message>
<xml_diff>
--- a/Selenium with CSharp/Selenium with CSharp/TestData2.xlsx
+++ b/Selenium with CSharp/Selenium with CSharp/TestData2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed.mohamed\Documents\GitHub\Selenium-c-\Selenium with CSharp\Selenium with CSharp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93105C22-09EF-4413-9186-CD68392DB067}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F6B9D8-B098-4F49-A823-12008BB0E976}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Alignment Project Name</t>
   </si>
@@ -72,25 +72,16 @@
     <t>Cerner</t>
   </si>
   <si>
-    <t>Pharmacy_h8Sept</t>
-  </si>
-  <si>
-    <t>p199342232</t>
-  </si>
-  <si>
-    <t>Alignment Project 192</t>
-  </si>
-  <si>
-    <t>TestAutomation_8Septt</t>
-  </si>
-  <si>
-    <t>A224119933241</t>
-  </si>
-  <si>
-    <t>Facility_h224933552q</t>
-  </si>
-  <si>
-    <t>h224933552q</t>
+    <t>TestAuto_POC1</t>
+  </si>
+  <si>
+    <t>Facility_POC1</t>
+  </si>
+  <si>
+    <t>Pharmacy_POC1</t>
+  </si>
+  <si>
+    <t>AlignmentProject_POC1</t>
   </si>
 </sst>
 </file>
@@ -141,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -279,6 +270,17 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -317,9 +319,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -328,6 +327,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -647,20 +649,20 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="4" width="29.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" customWidth="1"/>
+    <col min="3" max="4" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" customWidth="1"/>
     <col min="6" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -668,7 +670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -676,7 +678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="14"/>
       <c r="C3" s="12"/>
@@ -686,11 +688,11 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -712,30 +714,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>17</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>15</v>
+      <c r="H5" s="18" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>